<commit_message>
Respond to use note comments from Ying.
</commit_message>
<xml_diff>
--- a/off_model_calculators/finalized_excel/GHG Calculator CBTP_9-25-18.xlsx
+++ b/off_model_calculators/finalized_excel/GHG Calculator CBTP_9-25-18.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wsponline-my.sharepoint.com/personal/john_helsel_wsp_com/Documents/SANDAG/RTP 2019/off_model_calculators/finalized_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helseljw\OneDrive - WSP O365\SANDAG\RTP 2019\off_model_calculators\finalized_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11616" tabRatio="771" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11616" tabRatio="771"/>
   </bookViews>
   <sheets>
     <sheet name="Use Notes" sheetId="67" r:id="rId1"/>
@@ -2247,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2295,7 +2295,7 @@
         <v>123</v>
       </c>
       <c r="D7" s="59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E7" s="54" t="s">
         <v>63</v>
@@ -2420,7 +2420,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" location="'Main Sheet'!A1" display="Main Sheet"/>
-    <hyperlink ref="D7" location="'Population Forecast'!A1" display="Population forecast"/>
+    <hyperlink ref="D7" location="'Main Sheet'!A1" display="Main Sheet"/>
     <hyperlink ref="D13" location="'Main Sheet'!A1" display="Main Sheet"/>
     <hyperlink ref="D17" location="'Emission Factors'!A1" display="Emission Factors"/>
   </hyperlinks>
@@ -2433,7 +2433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B30" sqref="B30:F30"/>
     </sheetView>
   </sheetViews>

</xml_diff>